<commit_message>
change color on blue
</commit_message>
<xml_diff>
--- a/converter/words.xlsx
+++ b/converter/words.xlsx
@@ -20,24 +20,84 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t xml:space="preserve">do one's best</t>
-  </si>
-  <si>
-    <t xml:space="preserve">делать все возможное, стараться изо всех сил</t>
-  </si>
-  <si>
-    <t xml:space="preserve">it's up to smd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">тебе решать, все зависит от...</t>
-  </si>
-  <si>
-    <t xml:space="preserve">keep a promise</t>
-  </si>
-  <si>
-    <t xml:space="preserve">держать слово, сдержать обещание</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+  <si>
+    <t xml:space="preserve">lead led led</t>
+  </si>
+  <si>
+    <t xml:space="preserve">вести</t>
+  </si>
+  <si>
+    <t xml:space="preserve">understand understood understood</t>
+  </si>
+  <si>
+    <t xml:space="preserve">понимать</t>
+  </si>
+  <si>
+    <t xml:space="preserve">watch watched watched</t>
+  </si>
+  <si>
+    <t xml:space="preserve">смотреть</t>
+  </si>
+  <si>
+    <t xml:space="preserve">follow followed followed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">следовать</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stop stopped stopped</t>
+  </si>
+  <si>
+    <t xml:space="preserve">останавливать</t>
+  </si>
+  <si>
+    <t xml:space="preserve">create created created</t>
+  </si>
+  <si>
+    <t xml:space="preserve">создавать</t>
+  </si>
+  <si>
+    <t xml:space="preserve">speak spoke spoken</t>
+  </si>
+  <si>
+    <t xml:space="preserve">говорить</t>
+  </si>
+  <si>
+    <t xml:space="preserve">read read read</t>
+  </si>
+  <si>
+    <t xml:space="preserve">читать</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spend spent spent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">тратить</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grow grew grown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">расти</t>
+  </si>
+  <si>
+    <t xml:space="preserve">open opened opened</t>
+  </si>
+  <si>
+    <t xml:space="preserve">открывать</t>
+  </si>
+  <si>
+    <t xml:space="preserve">walk walked walked</t>
+  </si>
+  <si>
+    <t xml:space="preserve">идти</t>
+  </si>
+  <si>
+    <t xml:space="preserve">win won won</t>
+  </si>
+  <si>
+    <t xml:space="preserve">побеждать</t>
   </si>
 </sst>
 </file>
@@ -138,19 +198,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.79"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -158,7 +218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -166,12 +226,92 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>